<commit_message>
Mulitplizität von Spielfigur und Spielbrett abgeändert
</commit_message>
<xml_diff>
--- a/China_Schach.xlsx
+++ b/China_Schach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Temp\gse2_chinesisches_schach\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\Desktop\Software Engineering\2. Semester\GSE2\Aufgaben\Brettspiel\gse2_chinesisches_schach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865771F9-9A71-4C0D-B782-42E7BE579BB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723DFDFA-C9AE-47A4-AD19-F53184B36E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Klassen" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Klassenkandidaten</t>
   </si>
@@ -421,10 +421,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -445,6 +441,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1614,21 +1614,21 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="3"/>
@@ -1637,18 +1637,18 @@
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1669,12 +1669,12 @@
       <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1689,14 +1689,14 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1706,19 +1706,19 @@
       <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="79.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="79.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>10</v>
       </c>
@@ -1728,12 +1728,12 @@
       <c r="C9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="31" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
@@ -1743,12 +1743,12 @@
       <c r="C10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="29" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -1758,12 +1758,12 @@
       <c r="C11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>14</v>
       </c>
@@ -1773,12 +1773,12 @@
       <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="66" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
@@ -1788,12 +1788,12 @@
       <c r="C13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="29" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>16</v>
       </c>
@@ -1803,12 +1803,12 @@
       <c r="C14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="30" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>19</v>
       </c>
@@ -1833,19 +1833,19 @@
       <c r="C16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="29" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
+    <row r="17" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="66" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>20</v>
       </c>
@@ -1860,14 +1860,14 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>23</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="D20" s="21"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
@@ -1904,33 +1904,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="148" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="13.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="10.85546875" style="23"/>
+    <col min="1" max="1" width="34.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="13.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="10.88671875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="3"/>
@@ -1938,14 +1938,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -1962,8 +1962,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1979,7 +1979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1992,11 +1992,11 @@
       <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -2013,8 +2013,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -2030,7 +2030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>37</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -2166,28 +2166,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>23</v>
       </c>
@@ -2196,8 +2196,8 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
+    <row r="21" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="3"/>

</xml_diff>

<commit_message>
Changes to associations and class diagram
</commit_message>
<xml_diff>
--- a/China_Schach.xlsx
+++ b/China_Schach.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\Desktop\Software Engineering\2. Semester\GSE2\Aufgaben\Brettspiel\gse2_chinesisches_schach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723DFDFA-C9AE-47A4-AD19-F53184B36E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F272518C-1855-40BF-B634-AE4C2E0D91FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Klassenkandidaten</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Control-Klasse</t>
-  </si>
-  <si>
-    <t>Ist abgeleitet von</t>
   </si>
   <si>
     <t>Spielt auf</t>
@@ -1629,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
@@ -1649,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>3</v>
@@ -1670,7 +1667,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1707,7 +1704,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="32"/>
     </row>
@@ -1729,7 +1726,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -1744,7 +1741,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -1759,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -1774,7 +1771,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -1789,7 +1786,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="6"/>
     </row>
@@ -1804,7 +1801,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="6"/>
     </row>
@@ -1834,7 +1831,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="6"/>
     </row>
@@ -1878,7 +1875,7 @@
     </row>
     <row r="21" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -1904,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="148" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="148" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1928,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4" t="s">
@@ -2032,7 +2029,7 @@
     </row>
     <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -2049,7 +2046,7 @@
     </row>
     <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="11" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
@@ -2083,7 +2080,7 @@
     </row>
     <row r="12" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
@@ -2100,7 +2097,7 @@
     </row>
     <row r="13" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
@@ -2117,7 +2114,7 @@
     </row>
     <row r="14" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
@@ -2134,7 +2131,7 @@
     </row>
     <row r="15" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>17</v>
@@ -2151,7 +2148,7 @@
     </row>
     <row r="16" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -2198,7 +2195,7 @@
     </row>
     <row r="21" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>

</xml_diff>